<commit_message>
carpeta relacionada a los diagramas, métricas y gantt
En el repositorio se deja toda la documentación asociada al proyecto titulo
</commit_message>
<xml_diff>
--- a/Otros/cuadro metrica (version 5).xlsb.xlsx
+++ b/Otros/cuadro metrica (version 5).xlsb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7665" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7665" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="314">
   <si>
     <t>Sitauación Actual</t>
   </si>
@@ -976,9 +976,6 @@
     <t xml:space="preserve">quiero que la aplicación móvil permita trabajar en forma simultanea </t>
   </si>
   <si>
-    <t xml:space="preserve">La aplicación web debe permitor realizar busqueda por diferentes criterios </t>
-  </si>
-  <si>
     <t>para que se realicen tarjas en forma simultanea</t>
   </si>
   <si>
@@ -1353,25 +1350,28 @@
     <t>Desarrollar una aplicación Móvil que permita ingresar a la aplicación revisar las planificación asociadas al usuario tarjador, realizar el proceso consolidado y despacho para luego sincronizar con el servidor durante el proceso de cierre</t>
   </si>
   <si>
-    <t>falta de participación de los JOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se debera acudir a los terminales para pas reuniones </t>
-  </si>
-  <si>
-    <t xml:space="preserve">se fijara con anticipación las reuniones y JP rotara en los terminales </t>
-  </si>
-  <si>
-    <t>No se puede planificar</t>
-  </si>
-  <si>
     <t xml:space="preserve">sistema </t>
   </si>
   <si>
-    <t>se debe estandarizar el proceso de planificación</t>
-  </si>
-  <si>
-    <t>la planificación debe ser igal a la que se lleva en planilla</t>
+    <t xml:space="preserve">La aplicación web debe permitir realizar busqueda por diferentes criterios </t>
+  </si>
+  <si>
+    <t>poca experiencia en pruebas testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">planificar las pruebas a realizar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">comenzar con las pruebas de carga y usar herramientas web </t>
+  </si>
+  <si>
+    <t>No cerrar el proyecto en la fecha planificada.</t>
+  </si>
+  <si>
+    <t>se debera realizar revisión con los JOP antes de la presentación final y firma del cierre proyecto</t>
+  </si>
+  <si>
+    <t>planificar ronda de reuniones con los JOP con revisión del sistema.</t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="316">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2422,18 +2422,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -2449,18 +2443,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2507,10 +2491,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2529,271 +2509,16 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2807,37 +2532,337 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3056,6 +3081,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3344,6 +3370,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3464,6 +3491,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3538,6 +3566,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4171,16 +4200,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>702469</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>631032</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>428624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>145255</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>726282</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>609599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4210,7 +4239,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="702469" y="6738937"/>
+          <a:off x="10263188" y="2285999"/>
           <a:ext cx="3905250" cy="1859756"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4276,7 +4305,20 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:G20" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="B3:G20"/>
+  <autoFilter ref="B3:G20">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+        <filter val="10"/>
+        <filter val="16"/>
+        <filter val="2"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="6"/>
+        <filter val="7"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="Numero" dataDxfId="5"/>
     <tableColumn id="2" name="ROL" dataDxfId="4"/>
@@ -4644,32 +4686,32 @@
       <c r="F2" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="204" t="s">
+      <c r="G2" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="205"/>
-      <c r="I2" s="205" t="s">
+      <c r="H2" s="215"/>
+      <c r="I2" s="215" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="205"/>
-      <c r="K2" s="205" t="s">
+      <c r="J2" s="215"/>
+      <c r="K2" s="215" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="205"/>
-      <c r="M2" s="204" t="s">
+      <c r="L2" s="215"/>
+      <c r="M2" s="214" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="229"/>
+      <c r="N2" s="238"/>
       <c r="O2" s="102" t="s">
         <v>171</v>
       </c>
       <c r="P2" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="Q2" s="202" t="s">
+      <c r="Q2" s="212" t="s">
         <v>100</v>
       </c>
-      <c r="R2" s="203"/>
+      <c r="R2" s="213"/>
       <c r="S2" s="101" t="s">
         <v>96</v>
       </c>
@@ -4693,22 +4735,22 @@
       <c r="F3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="219" t="s">
+      <c r="G3" s="228" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="215" t="s">
+      <c r="H3" s="224" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="98" t="s">
         <v>74</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>254</v>
-      </c>
-      <c r="K3" s="225" t="s">
+        <v>253</v>
+      </c>
+      <c r="K3" s="234" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="222" t="s">
+      <c r="L3" s="231" t="s">
         <v>45</v>
       </c>
       <c r="M3" s="70">
@@ -4740,22 +4782,22 @@
       <c r="D4" s="59"/>
       <c r="E4" s="59"/>
       <c r="F4" s="61"/>
-      <c r="G4" s="220"/>
-      <c r="H4" s="216"/>
+      <c r="G4" s="229"/>
+      <c r="H4" s="225"/>
       <c r="I4" s="142" t="s">
         <v>88</v>
       </c>
       <c r="J4" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="226"/>
-      <c r="L4" s="223"/>
+      <c r="K4" s="235"/>
+      <c r="L4" s="232"/>
       <c r="M4" s="32"/>
       <c r="N4" s="72"/>
-      <c r="O4" s="240" t="s">
+      <c r="O4" s="209" t="s">
         <v>161</v>
       </c>
-      <c r="P4" s="240" t="s">
+      <c r="P4" s="209" t="s">
         <v>168</v>
       </c>
       <c r="Q4" s="32"/>
@@ -4769,31 +4811,31 @@
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
       <c r="F5" s="61"/>
-      <c r="G5" s="220"/>
-      <c r="H5" s="216"/>
-      <c r="I5" s="232" t="s">
+      <c r="G5" s="229"/>
+      <c r="H5" s="225"/>
+      <c r="I5" s="241" t="s">
         <v>75</v>
       </c>
-      <c r="J5" s="233" t="s">
+      <c r="J5" s="242" t="s">
         <v>140</v>
       </c>
-      <c r="K5" s="226"/>
-      <c r="L5" s="223"/>
-      <c r="M5" s="211">
+      <c r="K5" s="235"/>
+      <c r="L5" s="232"/>
+      <c r="M5" s="204">
         <v>2</v>
       </c>
-      <c r="N5" s="228" t="s">
+      <c r="N5" s="237" t="s">
         <v>95</v>
       </c>
-      <c r="O5" s="241"/>
-      <c r="P5" s="241"/>
+      <c r="O5" s="210"/>
+      <c r="P5" s="210"/>
       <c r="Q5" s="64" t="s">
         <v>102</v>
       </c>
       <c r="R5" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="S5" s="235" t="s">
+      <c r="S5" s="203" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4804,23 +4846,23 @@
       <c r="D6" s="59"/>
       <c r="E6" s="59"/>
       <c r="F6" s="61"/>
-      <c r="G6" s="220"/>
-      <c r="H6" s="216"/>
-      <c r="I6" s="232"/>
-      <c r="J6" s="233"/>
-      <c r="K6" s="226"/>
-      <c r="L6" s="223"/>
-      <c r="M6" s="211"/>
-      <c r="N6" s="228"/>
-      <c r="O6" s="241"/>
-      <c r="P6" s="241"/>
+      <c r="G6" s="229"/>
+      <c r="H6" s="225"/>
+      <c r="I6" s="241"/>
+      <c r="J6" s="242"/>
+      <c r="K6" s="235"/>
+      <c r="L6" s="232"/>
+      <c r="M6" s="204"/>
+      <c r="N6" s="237"/>
+      <c r="O6" s="210"/>
+      <c r="P6" s="210"/>
       <c r="Q6" s="64" t="s">
         <v>124</v>
       </c>
       <c r="R6" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="S6" s="235"/>
+      <c r="S6" s="203"/>
     </row>
     <row r="7" spans="1:19" ht="39" customHeight="1" thickBot="1">
       <c r="A7" s="56"/>
@@ -4829,23 +4871,23 @@
       <c r="D7" s="59"/>
       <c r="E7" s="59"/>
       <c r="F7" s="61"/>
-      <c r="G7" s="220"/>
-      <c r="H7" s="216"/>
+      <c r="G7" s="229"/>
+      <c r="H7" s="225"/>
       <c r="I7" s="99" t="s">
         <v>72</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="K7" s="226"/>
-      <c r="L7" s="223"/>
-      <c r="M7" s="211"/>
-      <c r="N7" s="228"/>
-      <c r="O7" s="242"/>
-      <c r="P7" s="242"/>
+      <c r="K7" s="235"/>
+      <c r="L7" s="232"/>
+      <c r="M7" s="204"/>
+      <c r="N7" s="237"/>
+      <c r="O7" s="211"/>
+      <c r="P7" s="211"/>
       <c r="Q7" s="64"/>
       <c r="R7" s="75"/>
-      <c r="S7" s="235"/>
+      <c r="S7" s="203"/>
     </row>
     <row r="8" spans="1:19" ht="79.5" thickBot="1">
       <c r="A8" s="56"/>
@@ -4854,16 +4896,16 @@
       <c r="D8" s="59"/>
       <c r="E8" s="59"/>
       <c r="F8" s="61"/>
-      <c r="G8" s="220"/>
-      <c r="H8" s="216"/>
+      <c r="G8" s="229"/>
+      <c r="H8" s="225"/>
       <c r="I8" s="55" t="s">
         <v>78</v>
       </c>
       <c r="J8" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="K8" s="226"/>
-      <c r="L8" s="223"/>
+      <c r="K8" s="235"/>
+      <c r="L8" s="232"/>
       <c r="M8" s="73">
         <v>3</v>
       </c>
@@ -4893,16 +4935,16 @@
       <c r="D9" s="59"/>
       <c r="E9" s="59"/>
       <c r="F9" s="61"/>
-      <c r="G9" s="220"/>
-      <c r="H9" s="216"/>
+      <c r="G9" s="229"/>
+      <c r="H9" s="225"/>
       <c r="I9" s="143" t="s">
         <v>73</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="K9" s="226"/>
-      <c r="L9" s="223"/>
+      <c r="K9" s="235"/>
+      <c r="L9" s="232"/>
       <c r="M9" s="64">
         <v>4</v>
       </c>
@@ -4932,16 +4974,16 @@
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
       <c r="F10" s="61"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="216"/>
+      <c r="G10" s="229"/>
+      <c r="H10" s="225"/>
       <c r="I10" s="144" t="s">
         <v>86</v>
       </c>
       <c r="J10" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="K10" s="226"/>
-      <c r="L10" s="223"/>
+      <c r="K10" s="235"/>
+      <c r="L10" s="232"/>
       <c r="M10" s="76">
         <v>5</v>
       </c>
@@ -4971,16 +5013,16 @@
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
       <c r="F11" s="61"/>
-      <c r="G11" s="220"/>
-      <c r="H11" s="216"/>
+      <c r="G11" s="229"/>
+      <c r="H11" s="225"/>
       <c r="I11" s="143" t="s">
         <v>79</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="K11" s="226"/>
-      <c r="L11" s="223"/>
+      <c r="K11" s="235"/>
+      <c r="L11" s="232"/>
       <c r="M11" s="78">
         <v>5</v>
       </c>
@@ -5008,16 +5050,16 @@
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
       <c r="F12" s="61"/>
-      <c r="G12" s="220"/>
-      <c r="H12" s="216"/>
+      <c r="G12" s="229"/>
+      <c r="H12" s="225"/>
       <c r="I12" s="87" t="s">
         <v>81</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="K12" s="226"/>
-      <c r="L12" s="223"/>
+      <c r="K12" s="235"/>
+      <c r="L12" s="232"/>
       <c r="M12" s="73">
         <v>7</v>
       </c>
@@ -5037,16 +5079,16 @@
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
       <c r="F13" s="61"/>
-      <c r="G13" s="220"/>
-      <c r="H13" s="216"/>
+      <c r="G13" s="229"/>
+      <c r="H13" s="225"/>
       <c r="I13" s="145" t="s">
         <v>84</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="K13" s="226"/>
-      <c r="L13" s="223"/>
+      <c r="K13" s="235"/>
+      <c r="L13" s="232"/>
       <c r="M13" s="80">
         <v>8</v>
       </c>
@@ -5066,16 +5108,16 @@
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
       <c r="F14" s="61"/>
-      <c r="G14" s="220"/>
-      <c r="H14" s="216"/>
+      <c r="G14" s="229"/>
+      <c r="H14" s="225"/>
       <c r="I14" s="146" t="s">
         <v>85</v>
       </c>
       <c r="J14" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="K14" s="227"/>
-      <c r="L14" s="224"/>
+      <c r="K14" s="236"/>
+      <c r="L14" s="233"/>
       <c r="M14" s="73">
         <v>9</v>
       </c>
@@ -5095,13 +5137,13 @@
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
       <c r="F15" s="61"/>
-      <c r="G15" s="220"/>
-      <c r="H15" s="217"/>
+      <c r="G15" s="229"/>
+      <c r="H15" s="226"/>
       <c r="I15" s="147" t="s">
         <v>115</v>
       </c>
       <c r="J15" s="94" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K15" s="44" t="s">
         <v>92</v>
@@ -5136,8 +5178,8 @@
       <c r="D16" s="59"/>
       <c r="E16" s="59"/>
       <c r="F16" s="61"/>
-      <c r="G16" s="221"/>
-      <c r="H16" s="218"/>
+      <c r="G16" s="230"/>
+      <c r="H16" s="227"/>
       <c r="I16" s="144" t="s">
         <v>113</v>
       </c>
@@ -5145,10 +5187,10 @@
         <v>112</v>
       </c>
       <c r="K16" s="48" t="s">
+        <v>267</v>
+      </c>
+      <c r="L16" s="69" t="s">
         <v>268</v>
-      </c>
-      <c r="L16" s="69" t="s">
-        <v>269</v>
       </c>
       <c r="M16" s="66">
         <v>11</v>
@@ -5264,9 +5306,9 @@
         <v>27</v>
       </c>
       <c r="G19" s="66" t="s">
-        <v>250</v>
-      </c>
-      <c r="H19" s="230" t="s">
+        <v>249</v>
+      </c>
+      <c r="H19" s="239" t="s">
         <v>7</v>
       </c>
       <c r="I19" s="146" t="s">
@@ -5293,7 +5335,7 @@
       <c r="E20" s="95"/>
       <c r="F20" s="96"/>
       <c r="G20" s="97"/>
-      <c r="H20" s="231"/>
+      <c r="H20" s="240"/>
       <c r="I20" s="144" t="s">
         <v>83</v>
       </c>
@@ -5315,16 +5357,16 @@
       <c r="S20" s="53"/>
     </row>
     <row r="21" spans="1:19" ht="90" customHeight="1">
-      <c r="A21" s="209" t="s">
-        <v>251</v>
-      </c>
-      <c r="B21" s="210"/>
-      <c r="C21" s="210"/>
-      <c r="D21" s="210"/>
-      <c r="E21" s="210"/>
-      <c r="F21" s="210"/>
-      <c r="G21" s="210"/>
-      <c r="H21" s="206" t="s">
+      <c r="A21" s="219" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="220"/>
+      <c r="C21" s="220"/>
+      <c r="D21" s="220"/>
+      <c r="E21" s="220"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="220"/>
+      <c r="H21" s="216" t="s">
         <v>9</v>
       </c>
       <c r="I21" s="142" t="s">
@@ -5335,35 +5377,35 @@
       </c>
       <c r="K21" s="64"/>
       <c r="L21" s="75"/>
-      <c r="M21" s="236">
+      <c r="M21" s="205">
         <v>12</v>
       </c>
-      <c r="N21" s="238" t="s">
+      <c r="N21" s="207" t="s">
         <v>136</v>
       </c>
-      <c r="O21" s="240" t="s">
+      <c r="O21" s="209" t="s">
         <v>164</v>
       </c>
-      <c r="P21" s="240" t="s">
+      <c r="P21" s="209" t="s">
         <v>169</v>
       </c>
       <c r="Q21" s="62"/>
       <c r="R21" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="S21" s="234" t="s">
+      <c r="S21" s="202" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="211"/>
-      <c r="B22" s="212"/>
-      <c r="C22" s="212"/>
-      <c r="D22" s="212"/>
-      <c r="E22" s="212"/>
-      <c r="F22" s="212"/>
-      <c r="G22" s="212"/>
-      <c r="H22" s="207"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="221"/>
+      <c r="C22" s="221"/>
+      <c r="D22" s="221"/>
+      <c r="E22" s="221"/>
+      <c r="F22" s="221"/>
+      <c r="G22" s="221"/>
+      <c r="H22" s="217"/>
       <c r="I22" s="99" t="s">
         <v>77</v>
       </c>
@@ -5372,25 +5414,25 @@
       </c>
       <c r="K22" s="64"/>
       <c r="L22" s="75"/>
-      <c r="M22" s="237"/>
-      <c r="N22" s="239"/>
-      <c r="O22" s="241"/>
-      <c r="P22" s="241"/>
+      <c r="M22" s="206"/>
+      <c r="N22" s="208"/>
+      <c r="O22" s="210"/>
+      <c r="P22" s="210"/>
       <c r="Q22" s="64"/>
       <c r="R22" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="S22" s="235"/>
+      <c r="S22" s="203"/>
     </row>
     <row r="23" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A23" s="211"/>
-      <c r="B23" s="212"/>
-      <c r="C23" s="212"/>
-      <c r="D23" s="212"/>
-      <c r="E23" s="212"/>
-      <c r="F23" s="212"/>
-      <c r="G23" s="212"/>
-      <c r="H23" s="207"/>
+      <c r="A23" s="204"/>
+      <c r="B23" s="221"/>
+      <c r="C23" s="221"/>
+      <c r="D23" s="221"/>
+      <c r="E23" s="221"/>
+      <c r="F23" s="221"/>
+      <c r="G23" s="221"/>
+      <c r="H23" s="217"/>
       <c r="I23" s="149" t="s">
         <v>80</v>
       </c>
@@ -5401,21 +5443,21 @@
       <c r="L23" s="79"/>
       <c r="M23" s="78"/>
       <c r="N23" s="79"/>
-      <c r="O23" s="242"/>
-      <c r="P23" s="242"/>
+      <c r="O23" s="211"/>
+      <c r="P23" s="211"/>
       <c r="Q23" s="78"/>
       <c r="R23" s="79"/>
       <c r="S23" s="54"/>
     </row>
     <row r="24" spans="1:19" ht="133.5" customHeight="1" thickBot="1">
-      <c r="A24" s="213"/>
-      <c r="B24" s="214"/>
-      <c r="C24" s="214"/>
-      <c r="D24" s="214"/>
-      <c r="E24" s="214"/>
-      <c r="F24" s="214"/>
-      <c r="G24" s="214"/>
-      <c r="H24" s="208"/>
+      <c r="A24" s="222"/>
+      <c r="B24" s="223"/>
+      <c r="C24" s="223"/>
+      <c r="D24" s="223"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="223"/>
+      <c r="H24" s="218"/>
       <c r="I24" s="55" t="s">
         <v>117</v>
       </c>
@@ -5486,15 +5528,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="S21:S22"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="S5:S7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="P21:P23"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="H21:H24"/>
@@ -5510,6 +5543,15 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="S21:S22"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="P21:P23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5520,7 +5562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:G10"/>
     </sheetView>
   </sheetViews>
@@ -5557,7 +5599,7 @@
     </row>
     <row r="3" spans="2:10" ht="29.25" customHeight="1">
       <c r="B3" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -5606,10 +5648,10 @@
         <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -5629,13 +5671,13 @@
         <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>24</v>
@@ -5652,7 +5694,7 @@
         <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
@@ -5695,7 +5737,7 @@
     </row>
     <row r="9" spans="2:10" ht="60">
       <c r="B9" s="127" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -5718,7 +5760,7 @@
     </row>
     <row r="10" spans="2:10" ht="60">
       <c r="B10" s="127" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -5807,7 +5849,7 @@
     </row>
     <row r="18" spans="2:7" ht="30">
       <c r="B18" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>0</v>
@@ -5830,13 +5872,13 @@
         <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>24</v>
@@ -5850,10 +5892,10 @@
         <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>11</v>
@@ -5867,7 +5909,7 @@
     </row>
     <row r="23" spans="2:7" ht="30">
       <c r="B23" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>0</v>
@@ -5907,7 +5949,7 @@
     </row>
     <row r="25" spans="2:7" ht="60">
       <c r="B25" s="127" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
@@ -5927,7 +5969,7 @@
     </row>
     <row r="26" spans="2:7" ht="60">
       <c r="B26" s="127" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
@@ -5946,13 +5988,13 @@
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="D27" s="171"/>
+      <c r="D27" s="164"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="171"/>
+      <c r="D28" s="164"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="D29" s="171"/>
+      <c r="D29" s="164"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5976,60 +6018,60 @@
   <sheetData>
     <row r="3" spans="3:5" ht="15.75" thickBot="1"/>
     <row r="4" spans="3:5" ht="34.5" customHeight="1" thickBot="1">
-      <c r="C4" s="288" t="s">
+      <c r="C4" s="191" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="193" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="191" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="23.25" customHeight="1">
+      <c r="C5" s="246" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" s="194" t="s">
+        <v>294</v>
+      </c>
+      <c r="E5" s="249" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="C6" s="247"/>
+      <c r="D6" s="197" t="s">
+        <v>295</v>
+      </c>
+      <c r="E6" s="250"/>
+    </row>
+    <row r="7" spans="3:5" ht="25.5" customHeight="1" thickBot="1">
+      <c r="C7" s="192" t="s">
         <v>298</v>
       </c>
-      <c r="D4" s="292" t="s">
-        <v>297</v>
-      </c>
-      <c r="E4" s="288" t="s">
+      <c r="D7" s="196" t="s">
+        <v>299</v>
+      </c>
+      <c r="E7" s="243" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="23.25" customHeight="1">
-      <c r="C5" s="289" t="s">
-        <v>294</v>
-      </c>
-      <c r="D5" s="293" t="s">
-        <v>295</v>
-      </c>
-      <c r="E5" s="296" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="C6" s="297"/>
-      <c r="D6" s="298" t="s">
-        <v>296</v>
-      </c>
-      <c r="E6" s="299"/>
-    </row>
-    <row r="7" spans="3:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="C7" s="291" t="s">
-        <v>299</v>
-      </c>
-      <c r="D7" s="295" t="s">
+    <row r="8" spans="3:5" ht="24.75" customHeight="1">
+      <c r="C8" s="246" t="s">
         <v>300</v>
       </c>
-      <c r="E7" s="300" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" ht="24.75" customHeight="1">
-      <c r="C8" s="289" t="s">
+      <c r="D8" s="194" t="s">
         <v>301</v>
       </c>
-      <c r="D8" s="293" t="s">
+      <c r="E8" s="244"/>
+    </row>
+    <row r="9" spans="3:5" ht="23.25" customHeight="1" thickBot="1">
+      <c r="C9" s="248"/>
+      <c r="D9" s="195" t="s">
         <v>302</v>
       </c>
-      <c r="E8" s="301"/>
-    </row>
-    <row r="9" spans="3:5" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C9" s="290"/>
-      <c r="D9" s="294" t="s">
-        <v>303</v>
-      </c>
-      <c r="E9" s="302"/>
+      <c r="E9" s="245"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6047,7 +6089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B44" sqref="B44:I46"/>
     </sheetView>
   </sheetViews>
@@ -6135,7 +6177,7 @@
       <c r="F4" s="9">
         <v>3</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="303">
         <v>9</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -6158,13 +6200,13 @@
         <v>41</v>
       </c>
       <c r="E5" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F5" s="9">
+        <v>2</v>
+      </c>
+      <c r="G5" s="201">
         <v>3</v>
-      </c>
-      <c r="G5" s="9">
-        <v>6</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>160</v>
@@ -6191,7 +6233,7 @@
       <c r="F6" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="303">
         <v>7</v>
       </c>
       <c r="H6" s="11" t="s">
@@ -6219,7 +6261,7 @@
       <c r="F7" s="9">
         <v>3</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="303">
         <v>8</v>
       </c>
       <c r="H7" s="11" t="s">
@@ -6247,7 +6289,7 @@
       <c r="F8" s="9">
         <v>3</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="300">
         <v>6</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -6275,7 +6317,7 @@
       <c r="F9" s="128">
         <v>2</v>
       </c>
-      <c r="G9" s="128">
+      <c r="G9" s="302">
         <v>7</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -6303,7 +6345,7 @@
       <c r="F10" s="128">
         <v>3</v>
       </c>
-      <c r="G10" s="128">
+      <c r="G10" s="302">
         <v>9</v>
       </c>
       <c r="H10" s="126" t="s">
@@ -6315,29 +6357,29 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="60">
-      <c r="B11" s="179">
+      <c r="B11" s="169">
         <v>8</v>
       </c>
       <c r="C11" s="139" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" s="180" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" s="170" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="181">
+      <c r="E11" s="171">
         <v>3</v>
       </c>
-      <c r="F11" s="182">
+      <c r="F11" s="172">
         <v>2</v>
       </c>
-      <c r="G11" s="182">
+      <c r="G11" s="301">
         <v>8</v>
       </c>
-      <c r="H11" s="183" t="s">
-        <v>267</v>
+      <c r="H11" s="173" t="s">
+        <v>266</v>
       </c>
       <c r="I11" s="139" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="75">
@@ -6345,7 +6387,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="129" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>41</v>
@@ -6356,17 +6398,68 @@
       <c r="F12" s="9">
         <v>3</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="200">
         <v>9</v>
       </c>
       <c r="H12" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I12" s="129" t="s">
         <v>281</v>
       </c>
-      <c r="I12" s="129" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="43.5" customHeight="1"/>
+    </row>
+    <row r="13" spans="1:19" ht="43.5" customHeight="1">
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="129" t="s">
+        <v>308</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="8">
+        <v>4</v>
+      </c>
+      <c r="F13" s="9">
+        <v>6</v>
+      </c>
+      <c r="G13" s="200">
+        <v>9</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="I13" s="198" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="48">
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="199" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3</v>
+      </c>
+      <c r="G14" s="300">
+        <v>3</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
     <row r="16" spans="1:19">
       <c r="S16" s="15"/>
     </row>
@@ -6400,7 +6493,7 @@
       <c r="B32" s="12">
         <v>2</v>
       </c>
-      <c r="C32" s="184" t="s">
+      <c r="C32" s="174" t="s">
         <v>159</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -6426,7 +6519,7 @@
       <c r="B33" s="12">
         <v>3</v>
       </c>
-      <c r="C33" s="184" t="s">
+      <c r="C33" s="174" t="s">
         <v>119</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -6452,8 +6545,8 @@
       <c r="B34" s="12">
         <v>8</v>
       </c>
-      <c r="C34" s="185" t="s">
-        <v>266</v>
+      <c r="C34" s="175" t="s">
+        <v>265</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>133</v>
@@ -6468,18 +6561,18 @@
         <v>8</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I34" s="129" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="75">
       <c r="B35" s="12">
         <v>9</v>
       </c>
-      <c r="C35" s="185" t="s">
-        <v>279</v>
+      <c r="C35" s="175" t="s">
+        <v>278</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>41</v>
@@ -6494,10 +6587,10 @@
         <v>9</v>
       </c>
       <c r="H35" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I35" s="129" t="s">
         <v>281</v>
-      </c>
-      <c r="I35" s="129" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="30">
@@ -6528,10 +6621,10 @@
     </row>
     <row r="45" spans="2:9" ht="45">
       <c r="B45" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C45" s="129" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>38</v>
@@ -6542,40 +6635,40 @@
       <c r="F45" s="9">
         <v>6</v>
       </c>
-      <c r="G45" s="305">
+      <c r="G45" s="200">
         <v>9</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="I45" s="303" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="46" spans="2:9" ht="45">
+      <c r="I45" s="198" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="48">
       <c r="B46" s="12">
-        <v>11</v>
-      </c>
-      <c r="C46" s="304" t="s">
-        <v>310</v>
+        <v>12</v>
+      </c>
+      <c r="C46" s="199" t="s">
+        <v>311</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E46" s="8">
         <v>1</v>
       </c>
       <c r="F46" s="9">
-        <v>2</v>
-      </c>
-      <c r="G46" s="306">
         <v>3</v>
       </c>
+      <c r="G46" s="300">
+        <v>3</v>
+      </c>
       <c r="H46" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="I46" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="I46" s="129" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -6730,10 +6823,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K26"/>
+  <dimension ref="B3:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6747,22 +6840,22 @@
   <sheetData>
     <row r="3" spans="2:11">
       <c r="B3" s="134" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="135" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="135" t="s">
+      <c r="D3" s="136" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="E3" s="136" t="s">
         <v>217</v>
-      </c>
-      <c r="E3" s="136" t="s">
-        <v>218</v>
       </c>
       <c r="F3" s="151" t="s">
         <v>171</v>
       </c>
       <c r="G3" s="153" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="30">
@@ -6779,7 +6872,7 @@
         <v>174</v>
       </c>
       <c r="F4" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G4" s="154">
         <v>8</v>
@@ -6793,19 +6886,19 @@
         <v>172</v>
       </c>
       <c r="D5" s="129" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E5" s="129" t="s">
         <v>175</v>
       </c>
       <c r="F5" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G5" s="154">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="30">
+    <row r="6" spans="2:11" ht="30" hidden="1">
       <c r="B6" s="132">
         <v>3</v>
       </c>
@@ -6813,13 +6906,13 @@
         <v>172</v>
       </c>
       <c r="D6" s="130" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="129" t="s">
         <v>176</v>
       </c>
       <c r="F6" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G6" s="154">
         <v>7</v>
@@ -6839,7 +6932,7 @@
         <v>178</v>
       </c>
       <c r="F7" s="133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G7" s="154">
         <v>5</v>
@@ -6859,7 +6952,7 @@
         <v>187</v>
       </c>
       <c r="F8" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G8" s="154">
         <v>8</v>
@@ -6879,7 +6972,7 @@
         <v>189</v>
       </c>
       <c r="F9" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G9" s="154">
         <v>8</v>
@@ -6899,13 +6992,13 @@
         <v>191</v>
       </c>
       <c r="F10" s="133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G10" s="154">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30">
+    <row r="11" spans="2:11" ht="30" hidden="1">
       <c r="B11" s="132">
         <v>8</v>
       </c>
@@ -6919,13 +7012,13 @@
         <v>193</v>
       </c>
       <c r="F11" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G11" s="154">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="30">
+    <row r="12" spans="2:11" ht="30" hidden="1">
       <c r="B12" s="132">
         <v>9</v>
       </c>
@@ -6936,10 +7029,10 @@
         <v>195</v>
       </c>
       <c r="E12" s="129" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G12" s="154">
         <v>8</v>
@@ -6953,19 +7046,19 @@
         <v>194</v>
       </c>
       <c r="D13" s="129" t="s">
-        <v>196</v>
+        <v>307</v>
       </c>
       <c r="E13" s="129" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F13" s="133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G13" s="154">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="30">
+    <row r="14" spans="2:11" ht="30" hidden="1">
       <c r="B14" s="132">
         <v>11</v>
       </c>
@@ -6973,20 +7066,20 @@
         <v>194</v>
       </c>
       <c r="D14" s="129" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E14" s="129" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G14" s="154">
         <v>7</v>
       </c>
       <c r="K14" s="152"/>
     </row>
-    <row r="15" spans="2:11" ht="30">
+    <row r="15" spans="2:11" ht="30" hidden="1">
       <c r="B15" s="132">
         <v>12</v>
       </c>
@@ -6994,39 +7087,39 @@
         <v>194</v>
       </c>
       <c r="D15" s="129" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="129" t="s">
         <v>200</v>
       </c>
-      <c r="E15" s="129" t="s">
-        <v>201</v>
-      </c>
       <c r="F15" s="133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G15" s="154">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="30">
+    <row r="16" spans="2:11" ht="30" hidden="1">
       <c r="B16" s="132">
         <v>13</v>
       </c>
       <c r="C16" s="131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D16" s="129" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="129" t="s">
         <v>202</v>
       </c>
-      <c r="E16" s="129" t="s">
-        <v>203</v>
-      </c>
       <c r="F16" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G16" s="154">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30">
+    <row r="17" spans="2:7" ht="30" hidden="1">
       <c r="B17" s="132">
         <v>14</v>
       </c>
@@ -7034,33 +7127,33 @@
         <v>194</v>
       </c>
       <c r="D17" s="129" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E17" s="129" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F17" s="133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G17" s="154">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30">
+    <row r="18" spans="2:7" ht="30" hidden="1">
       <c r="B18" s="132">
         <v>15</v>
       </c>
       <c r="C18" s="131" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E18" s="129" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F18" s="133" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G18" s="154">
         <v>6</v>
@@ -7074,33 +7167,33 @@
         <v>172</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E19" s="129" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="133" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G19" s="154">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" hidden="1">
       <c r="B20" s="137">
         <v>17</v>
       </c>
       <c r="C20" s="138" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D20" s="139" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E20" s="139" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F20" s="140" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G20" s="154">
         <v>7</v>
@@ -7111,18 +7204,6 @@
     </row>
     <row r="22" spans="2:7">
       <c r="D22" s="125"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="D23" s="125"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="D24" s="125"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="D25" s="125"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="D26" s="125"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7137,379 +7218,391 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I22"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="42.5703125" customWidth="1"/>
-    <col min="5" max="5" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="46.28515625" customWidth="1"/>
-    <col min="8" max="8" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" customWidth="1"/>
+    <col min="8" max="8" width="52.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="14" max="14" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="3" spans="1:9" s="196" customFormat="1" ht="42.75" customHeight="1" thickBot="1">
-      <c r="B3" s="197" t="s">
+    <row r="3" spans="1:9" s="182" customFormat="1" ht="42.75" customHeight="1" thickBot="1">
+      <c r="B3" s="183" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="183" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="183" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="183" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="184" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="185" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="186" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="187" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="47.25">
+      <c r="B4" s="176" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="159" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="197" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="197" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="197" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="198" t="s">
-        <v>166</v>
-      </c>
-      <c r="G3" s="199" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="200" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="201" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="47.25">
-      <c r="B4" s="186" t="s">
-        <v>287</v>
-      </c>
-      <c r="C4" s="165" t="s">
+      <c r="D4" s="159" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="160"/>
+      <c r="F4" s="287" t="s">
+        <v>291</v>
+      </c>
+      <c r="G4" s="161"/>
+      <c r="H4" s="304" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="155" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="31.5">
+      <c r="B5" s="177"/>
+      <c r="C5" s="286" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="165" t="s">
-        <v>264</v>
-      </c>
-      <c r="E4" s="166"/>
-      <c r="F4" s="243" t="s">
+      <c r="D5" s="190"/>
+      <c r="E5" s="274" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" s="288"/>
+      <c r="G5" s="162" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" s="305" t="s">
+        <v>222</v>
+      </c>
+      <c r="I5" s="156" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1">
+      <c r="B6" s="177"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="274"/>
+      <c r="F6" s="288"/>
+      <c r="G6" s="272" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" s="305" t="s">
+        <v>223</v>
+      </c>
+      <c r="I6" s="156" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="32.25" thickBot="1">
+      <c r="B7" s="177"/>
+      <c r="C7" s="163" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" s="163"/>
+      <c r="E7" s="290"/>
+      <c r="F7" s="289"/>
+      <c r="G7" s="291"/>
+      <c r="H7" s="306" t="s">
+        <v>224</v>
+      </c>
+      <c r="I7" s="157" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
+      <c r="B8" s="177"/>
+      <c r="C8" s="277" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="188"/>
+      <c r="E8" s="292" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="269" t="s">
         <v>292</v>
       </c>
-      <c r="G4" s="167"/>
-      <c r="H4" s="163" t="s">
-        <v>222</v>
-      </c>
-      <c r="I4" s="159" t="s">
+      <c r="G8" s="294" t="s">
+        <v>240</v>
+      </c>
+      <c r="H8" s="307" t="s">
+        <v>225</v>
+      </c>
+      <c r="I8" s="155" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="49.5" customHeight="1" thickBot="1">
+      <c r="B9" s="178"/>
+      <c r="C9" s="278"/>
+      <c r="D9" s="189" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="293"/>
+      <c r="F9" s="293"/>
+      <c r="G9" s="295"/>
+      <c r="H9" s="308" t="s">
+        <v>226</v>
+      </c>
+      <c r="I9" s="157" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" customHeight="1">
+      <c r="B10" s="254" t="s">
+        <v>285</v>
+      </c>
+      <c r="C10" s="279" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" s="165"/>
+      <c r="E10" s="275" t="s">
+        <v>275</v>
+      </c>
+      <c r="F10" s="273" t="s">
+        <v>292</v>
+      </c>
+      <c r="G10" s="271" t="s">
+        <v>241</v>
+      </c>
+      <c r="H10" s="304" t="s">
+        <v>254</v>
+      </c>
+      <c r="I10" s="155" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
+      <c r="B11" s="254"/>
+      <c r="C11" s="280"/>
+      <c r="D11" s="166" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="276"/>
+      <c r="F11" s="274"/>
+      <c r="G11" s="272"/>
+      <c r="H11" s="305" t="s">
+        <v>227</v>
+      </c>
+      <c r="I11" s="156" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="32.25" customHeight="1" thickBot="1">
+      <c r="B12" s="255"/>
+      <c r="C12" s="281"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="276"/>
+      <c r="F12" s="274"/>
+      <c r="G12" s="272"/>
+      <c r="H12" s="305" t="s">
+        <v>228</v>
+      </c>
+      <c r="I12" s="157" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A13" s="158"/>
+      <c r="B13" s="284" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="282" t="s">
+        <v>270</v>
+      </c>
+      <c r="D13" s="167"/>
+      <c r="E13" s="219" t="s">
+        <v>276</v>
+      </c>
+      <c r="F13" s="269" t="s">
+        <v>292</v>
+      </c>
+      <c r="G13" s="267" t="s">
+        <v>271</v>
+      </c>
+      <c r="H13" s="309" t="s">
+        <v>229</v>
+      </c>
+      <c r="I13" s="155" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
+      <c r="B14" s="285"/>
+      <c r="C14" s="283"/>
+      <c r="D14" s="168" t="s">
+        <v>279</v>
+      </c>
+      <c r="E14" s="204"/>
+      <c r="F14" s="270"/>
+      <c r="G14" s="268"/>
+      <c r="H14" s="310" t="s">
+        <v>230</v>
+      </c>
+      <c r="I14" s="156" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1">
+      <c r="B15" s="311"/>
+      <c r="C15" s="312"/>
+      <c r="D15" s="313"/>
+      <c r="E15" s="222"/>
+      <c r="F15" s="293"/>
+      <c r="G15" s="314"/>
+      <c r="H15" s="315" t="s">
+        <v>231</v>
+      </c>
+      <c r="I15" s="179" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="251" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" s="264" t="s">
+        <v>255</v>
+      </c>
+      <c r="D16" s="259" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" s="256" t="s">
+        <v>277</v>
+      </c>
+      <c r="F16" s="259" t="s">
+        <v>291</v>
+      </c>
+      <c r="G16" s="256" t="s">
+        <v>283</v>
+      </c>
+      <c r="H16" s="155" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="180"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="252"/>
+      <c r="C17" s="265"/>
+      <c r="D17" s="262"/>
+      <c r="E17" s="257"/>
+      <c r="F17" s="260"/>
+      <c r="G17" s="257"/>
+      <c r="H17" s="156" t="s">
+        <v>257</v>
+      </c>
+      <c r="I17" s="181" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="252"/>
+      <c r="C18" s="265"/>
+      <c r="D18" s="262"/>
+      <c r="E18" s="257"/>
+      <c r="F18" s="260"/>
+      <c r="G18" s="257"/>
+      <c r="H18" s="296" t="s">
+        <v>258</v>
+      </c>
+      <c r="I18" s="297" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
-      <c r="B5" s="187"/>
-      <c r="C5" s="264" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="174"/>
-      <c r="E5" s="246" t="s">
-        <v>275</v>
-      </c>
-      <c r="F5" s="244"/>
-      <c r="G5" s="168" t="s">
-        <v>239</v>
-      </c>
-      <c r="H5" s="164" t="s">
-        <v>223</v>
-      </c>
-      <c r="I5" s="160" t="s">
+    <row r="19" spans="2:9">
+      <c r="B19" s="252"/>
+      <c r="C19" s="265"/>
+      <c r="D19" s="262"/>
+      <c r="E19" s="257"/>
+      <c r="F19" s="260"/>
+      <c r="G19" s="257"/>
+      <c r="H19" s="156" t="s">
+        <v>259</v>
+      </c>
+      <c r="I19" s="181" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="252"/>
+      <c r="C20" s="265"/>
+      <c r="D20" s="262"/>
+      <c r="E20" s="257"/>
+      <c r="F20" s="260"/>
+      <c r="G20" s="257"/>
+      <c r="H20" s="156" t="s">
+        <v>260</v>
+      </c>
+      <c r="I20" s="181"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="252"/>
+      <c r="C21" s="265"/>
+      <c r="D21" s="262"/>
+      <c r="E21" s="257"/>
+      <c r="F21" s="260"/>
+      <c r="G21" s="257"/>
+      <c r="H21" s="296" t="s">
+        <v>261</v>
+      </c>
+      <c r="I21" s="297" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1">
-      <c r="B6" s="187"/>
-      <c r="C6" s="264"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="246"/>
-      <c r="F6" s="244"/>
-      <c r="G6" s="248" t="s">
-        <v>240</v>
-      </c>
-      <c r="H6" s="164" t="s">
-        <v>224</v>
-      </c>
-      <c r="I6" s="160" t="s">
+    <row r="22" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B22" s="253"/>
+      <c r="C22" s="266"/>
+      <c r="D22" s="263"/>
+      <c r="E22" s="258"/>
+      <c r="F22" s="261"/>
+      <c r="G22" s="258"/>
+      <c r="H22" s="298" t="s">
+        <v>262</v>
+      </c>
+      <c r="I22" s="299" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="32.25" thickBot="1">
-      <c r="B7" s="187"/>
-      <c r="C7" s="169" t="s">
-        <v>233</v>
-      </c>
-      <c r="D7" s="169"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="245"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="170" t="s">
-        <v>225</v>
-      </c>
-      <c r="I7" s="161" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75">
-      <c r="B8" s="187"/>
-      <c r="C8" s="255" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="172"/>
-      <c r="E8" s="250" t="s">
-        <v>274</v>
-      </c>
-      <c r="F8" s="252" t="s">
-        <v>293</v>
-      </c>
-      <c r="G8" s="253" t="s">
-        <v>241</v>
-      </c>
-      <c r="H8" s="155" t="s">
-        <v>226</v>
-      </c>
-      <c r="I8" s="159" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="49.5" customHeight="1" thickBot="1">
-      <c r="B9" s="188"/>
-      <c r="C9" s="256"/>
-      <c r="D9" s="173" t="s">
-        <v>270</v>
-      </c>
-      <c r="E9" s="251"/>
-      <c r="F9" s="251"/>
-      <c r="G9" s="254"/>
-      <c r="H9" s="156" t="s">
-        <v>227</v>
-      </c>
-      <c r="I9" s="161" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" customHeight="1">
-      <c r="B10" s="268" t="s">
-        <v>286</v>
-      </c>
-      <c r="C10" s="257" t="s">
-        <v>238</v>
-      </c>
-      <c r="D10" s="175"/>
-      <c r="E10" s="286" t="s">
-        <v>276</v>
-      </c>
-      <c r="F10" s="285" t="s">
-        <v>293</v>
-      </c>
-      <c r="G10" s="284" t="s">
-        <v>242</v>
-      </c>
-      <c r="H10" s="163" t="s">
-        <v>255</v>
-      </c>
-      <c r="I10" s="159" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
-      <c r="B11" s="268"/>
-      <c r="C11" s="258"/>
-      <c r="D11" s="176" t="s">
-        <v>283</v>
-      </c>
-      <c r="E11" s="287"/>
-      <c r="F11" s="246"/>
-      <c r="G11" s="248"/>
-      <c r="H11" s="164" t="s">
-        <v>228</v>
-      </c>
-      <c r="I11" s="160" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B12" s="269"/>
-      <c r="C12" s="259"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="287"/>
-      <c r="F12" s="246"/>
-      <c r="G12" s="248"/>
-      <c r="H12" s="164" t="s">
-        <v>229</v>
-      </c>
-      <c r="I12" s="161" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A13" s="162"/>
-      <c r="B13" s="262" t="s">
-        <v>285</v>
-      </c>
-      <c r="C13" s="260" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="177"/>
-      <c r="E13" s="209" t="s">
-        <v>277</v>
-      </c>
-      <c r="F13" s="252" t="s">
-        <v>293</v>
-      </c>
-      <c r="G13" s="281" t="s">
-        <v>272</v>
-      </c>
-      <c r="H13" s="157" t="s">
-        <v>230</v>
-      </c>
-      <c r="I13" s="159" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="B14" s="263"/>
-      <c r="C14" s="261"/>
-      <c r="D14" s="178" t="s">
-        <v>280</v>
-      </c>
-      <c r="E14" s="211"/>
-      <c r="F14" s="283"/>
-      <c r="G14" s="282"/>
-      <c r="H14" s="158" t="s">
-        <v>231</v>
-      </c>
-      <c r="I14" s="160" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B15" s="263"/>
-      <c r="C15" s="261"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="211"/>
-      <c r="F15" s="283"/>
-      <c r="G15" s="282"/>
-      <c r="H15" s="158" t="s">
-        <v>232</v>
-      </c>
-      <c r="I15" s="189" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="B16" s="265" t="s">
-        <v>287</v>
-      </c>
-      <c r="C16" s="278" t="s">
-        <v>256</v>
-      </c>
-      <c r="D16" s="273" t="s">
-        <v>273</v>
-      </c>
-      <c r="E16" s="270" t="s">
-        <v>278</v>
-      </c>
-      <c r="F16" s="273" t="s">
-        <v>292</v>
-      </c>
-      <c r="G16" s="270" t="s">
-        <v>284</v>
-      </c>
-      <c r="H16" s="159" t="s">
-        <v>257</v>
-      </c>
-      <c r="I16" s="190"/>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="266"/>
-      <c r="C17" s="279"/>
-      <c r="D17" s="276"/>
-      <c r="E17" s="271"/>
-      <c r="F17" s="274"/>
-      <c r="G17" s="271"/>
-      <c r="H17" s="160" t="s">
-        <v>258</v>
-      </c>
-      <c r="I17" s="191" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="266"/>
-      <c r="C18" s="279"/>
-      <c r="D18" s="276"/>
-      <c r="E18" s="271"/>
-      <c r="F18" s="274"/>
-      <c r="G18" s="271"/>
-      <c r="H18" s="193" t="s">
-        <v>259</v>
-      </c>
-      <c r="I18" s="192" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="266"/>
-      <c r="C19" s="279"/>
-      <c r="D19" s="276"/>
-      <c r="E19" s="271"/>
-      <c r="F19" s="274"/>
-      <c r="G19" s="271"/>
-      <c r="H19" s="160" t="s">
-        <v>260</v>
-      </c>
-      <c r="I19" s="191" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" s="266"/>
-      <c r="C20" s="279"/>
-      <c r="D20" s="276"/>
-      <c r="E20" s="271"/>
-      <c r="F20" s="274"/>
-      <c r="G20" s="271"/>
-      <c r="H20" s="160" t="s">
-        <v>261</v>
-      </c>
-      <c r="I20" s="191"/>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" s="266"/>
-      <c r="C21" s="279"/>
-      <c r="D21" s="276"/>
-      <c r="E21" s="271"/>
-      <c r="F21" s="274"/>
-      <c r="G21" s="271"/>
-      <c r="H21" s="193" t="s">
-        <v>262</v>
-      </c>
-      <c r="I21" s="192" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B22" s="267"/>
-      <c r="C22" s="280"/>
-      <c r="D22" s="277"/>
-      <c r="E22" s="272"/>
-      <c r="F22" s="275"/>
-      <c r="G22" s="272"/>
-      <c r="H22" s="194" t="s">
-        <v>263</v>
-      </c>
-      <c r="I22" s="195" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="B16:B22"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="G16:G22"/>
@@ -7523,17 +7616,6 @@
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="E10:E12"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>